<commit_message>
Base interface + neural teseract
</commit_message>
<xml_diff>
--- a/student1_checked.xlsx
+++ b/student1_checked.xlsx
@@ -14,63 +14,135 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>Ко ЗА</t>
-  </si>
-  <si>
-    <t>ША РФЫ</t>
-  </si>
-  <si>
-    <t>ВЕЛИКИЙ</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>ПЯТисСотТ</t>
-  </si>
-  <si>
-    <t>$375</t>
+    <t>13</t>
+  </si>
+  <si>
+    <t>КОГЧАВЕ</t>
+  </si>
+  <si>
+    <t>когда</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>ШАРФЫ</t>
+  </si>
+  <si>
+    <t>шарфы</t>
+  </si>
+  <si>
+    <t>ВЕЛЙКИЙ</t>
+  </si>
+  <si>
+    <t>величественной</t>
+  </si>
+  <si>
+    <t>ЗйГЛИтЪ</t>
+  </si>
+  <si>
+    <t>загладить</t>
+  </si>
+  <si>
+    <t>ПЯТИСоТу</t>
+  </si>
+  <si>
+    <t>пятисот</t>
+  </si>
+  <si>
+    <t>1375</t>
+  </si>
+  <si>
+    <t>16375</t>
+  </si>
+  <si>
+    <t>15</t>
   </si>
   <si>
     <t>135</t>
   </si>
   <si>
-    <t>44</t>
+    <t>11</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>12</t>
   </si>
   <si>
     <t>65</t>
   </si>
   <si>
-    <t>435</t>
+    <t>56</t>
+  </si>
+  <si>
+    <t>НААоЛГОТОЖЕ</t>
+  </si>
+  <si>
+    <t>надолгИИИтоже</t>
+  </si>
+  <si>
+    <t>2353</t>
+  </si>
+  <si>
+    <t>235</t>
+  </si>
+  <si>
+    <t>3477</t>
   </si>
   <si>
     <t>34</t>
   </si>
   <si>
-    <t>429</t>
-  </si>
-  <si>
-    <t>43</t>
+    <t>237</t>
+  </si>
+  <si>
+    <t>1237</t>
+  </si>
+  <si>
+    <t>137</t>
   </si>
   <si>
     <t>125</t>
   </si>
   <si>
-    <t>254</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>ПОМЕГАЕТ</t>
-  </si>
-  <si>
-    <t>2</t>
+    <t>123</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>234</t>
+  </si>
+  <si>
+    <t>265</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>рдМАВАЁТ</t>
+  </si>
+  <si>
+    <t>мешаетИИИпомогает</t>
+  </si>
+  <si>
+    <t>577</t>
+  </si>
+  <si>
+    <t>776</t>
+  </si>
+  <si>
+    <t>2746</t>
   </si>
 </sst>
 </file>
@@ -402,228 +474,324 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>26</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>28</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>33</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24">
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+        <v>38</v>
+      </c>
+      <c r="C24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="B25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26">
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
+        <v>41</v>
+      </c>
+      <c r="C26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:3">
       <c r="A28">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:3">
       <c r="A29">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:3">
       <c r="A30">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:3">
       <c r="A31">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:3">
       <c r="A32">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
≈ MCV, rotation undone
</commit_message>
<xml_diff>
--- a/student1_checked.xlsx
+++ b/student1_checked.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+  <si>
+    <t>15</t>
+  </si>
   <si>
     <t>13</t>
   </si>
   <si>
-    <t>КОйЗА</t>
+    <t>КоГАЛдзьооолсвоооц</t>
   </si>
   <si>
     <t>когда</t>
@@ -28,100 +31,124 @@
     <t>1</t>
   </si>
   <si>
-    <t>ШАРФЫ</t>
+    <t>шАРФЫбсооаесооьоУечоае</t>
   </si>
   <si>
     <t>шарфы</t>
   </si>
   <si>
-    <t>ВЕЛЙКЙЙ</t>
+    <t>ВЕЛИКИЙчаачЗЁвооьо</t>
   </si>
   <si>
     <t>величественной</t>
   </si>
   <si>
-    <t>ЗГЛАИтЪ</t>
+    <t>ЗАГААЁИТЬЪтчоть</t>
   </si>
   <si>
     <t>загладить</t>
   </si>
   <si>
-    <t>ПЭТМсоТ</t>
+    <t>ПЯтИСйЗЁ</t>
   </si>
   <si>
     <t>пятисот</t>
   </si>
   <si>
+    <t>13751</t>
+  </si>
+  <si>
+    <t>16375</t>
+  </si>
+  <si>
+    <t>13202</t>
+  </si>
+  <si>
+    <t>13511111</t>
+  </si>
+  <si>
+    <t>135</t>
+  </si>
+  <si>
+    <t>1111211</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>1211221</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>65491182221</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>НААдЛГотЁКЕЕоеЪБЁЁ</t>
+  </si>
+  <si>
+    <t>надолгИИИтоже</t>
+  </si>
+  <si>
+    <t>231215112</t>
+  </si>
+  <si>
+    <t>235</t>
+  </si>
+  <si>
+    <t>35522</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>1137582</t>
+  </si>
+  <si>
+    <t>1237</t>
+  </si>
+  <si>
+    <t>3522222</t>
+  </si>
+  <si>
+    <t>2355121222</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>232352221</t>
+  </si>
+  <si>
+    <t>234</t>
+  </si>
+  <si>
+    <t>261131</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
     <t>1315</t>
   </si>
   <si>
-    <t>16375</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>135</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>65</t>
-  </si>
-  <si>
-    <t>56</t>
-  </si>
-  <si>
-    <t>НААоЛГОТЛЖЕ</t>
-  </si>
-  <si>
-    <t>надолгИИИтоже</t>
-  </si>
-  <si>
-    <t>2353</t>
-  </si>
-  <si>
-    <t>235</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>1237</t>
-  </si>
-  <si>
-    <t>125</t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>237</t>
-  </si>
-  <si>
-    <t>234</t>
-  </si>
-  <si>
-    <t>26</t>
+    <t>1313</t>
+  </si>
+  <si>
+    <t>ПОмОГАЕТЦтПн</t>
+  </si>
+  <si>
+    <t>мешаетИИИпомогает</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
-    <t>рОМАГАЁТ</t>
-  </si>
-  <si>
-    <t>мешаетИИИпомогает</t>
-  </si>
-  <si>
-    <t>77</t>
+    <t>2761</t>
   </si>
   <si>
     <t>2746</t>
@@ -470,7 +497,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -478,21 +505,18 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -500,10 +524,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -511,10 +535,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -522,10 +546,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -533,10 +557,10 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -544,10 +568,10 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -555,10 +579,10 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -566,10 +590,10 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -577,10 +601,10 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -588,10 +612,10 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -599,10 +623,10 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -610,10 +634,10 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -621,10 +645,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -632,10 +656,10 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -643,10 +667,10 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -654,10 +678,10 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -665,10 +689,10 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -676,10 +700,10 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -687,10 +711,10 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -698,10 +722,10 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="C22" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -709,10 +733,10 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C23" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -720,21 +744,18 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25">
         <v>25</v>
       </c>
-      <c r="B25" t="s">
-        <v>32</v>
-      </c>
       <c r="C25" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -742,10 +763,10 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C26" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:3">

</xml_diff>